<commit_message>
updated 2013 class (thru Troy Williams)
</commit_message>
<xml_diff>
--- a/data/CollegeFootballQBs.xlsx
+++ b/data/CollegeFootballQBs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="62">
   <si>
     <t>Senior</t>
   </si>
@@ -184,6 +184,24 @@
   </si>
   <si>
     <t>Mason Rudolph</t>
+  </si>
+  <si>
+    <t>Max Browne</t>
+  </si>
+  <si>
+    <t>Christian Hackenberg</t>
+  </si>
+  <si>
+    <t>Shane Morris</t>
+  </si>
+  <si>
+    <t>Cooper Bateman</t>
+  </si>
+  <si>
+    <t>Kevin Olsen</t>
+  </si>
+  <si>
+    <t>Troy Williams</t>
   </si>
 </sst>
 </file>
@@ -533,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA43"/>
+  <dimension ref="A1:AA65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="AA42" sqref="AA42"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3126,6 +3144,1574 @@
       </c>
       <c r="AA43" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27">
+      <c r="A44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2">
+        <v>2012</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F44" s="1">
+        <v>14</v>
+      </c>
+      <c r="G44" s="1">
+        <v>277</v>
+      </c>
+      <c r="H44" s="1">
+        <v>377</v>
+      </c>
+      <c r="I44" s="1">
+        <v>4526</v>
+      </c>
+      <c r="J44" s="1">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="K44" s="1">
+        <v>16.3</v>
+      </c>
+      <c r="L44" s="1">
+        <v>323.3</v>
+      </c>
+      <c r="N44" s="1">
+        <v>49</v>
+      </c>
+      <c r="P44" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>80</v>
+      </c>
+      <c r="R44" s="1">
+        <v>147.4</v>
+      </c>
+      <c r="S44" s="1">
+        <v>67</v>
+      </c>
+      <c r="T44" s="1">
+        <v>15</v>
+      </c>
+      <c r="U44" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="V44" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="W44" s="1">
+        <v>17</v>
+      </c>
+      <c r="Y44" s="1">
+        <v>6</v>
+      </c>
+      <c r="Z44" s="1">
+        <v>14</v>
+      </c>
+      <c r="AA44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27">
+      <c r="A45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="1">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2">
+        <v>2011</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F45" s="1">
+        <v>14</v>
+      </c>
+      <c r="G45" s="1">
+        <v>288</v>
+      </c>
+      <c r="H45" s="1">
+        <v>409</v>
+      </c>
+      <c r="I45" s="1">
+        <v>4034</v>
+      </c>
+      <c r="J45" s="1">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="K45" s="1">
+        <v>14</v>
+      </c>
+      <c r="L45" s="1">
+        <v>288.10000000000002</v>
+      </c>
+      <c r="N45" s="1">
+        <v>45</v>
+      </c>
+      <c r="P45" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>82</v>
+      </c>
+      <c r="R45" s="1">
+        <v>131.4</v>
+      </c>
+      <c r="S45" s="1">
+        <v>42</v>
+      </c>
+      <c r="T45" s="1">
+        <v>221</v>
+      </c>
+      <c r="U45" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="V45" s="1">
+        <v>15.8</v>
+      </c>
+      <c r="W45" s="1">
+        <v>26</v>
+      </c>
+      <c r="Y45" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z45" s="1">
+        <v>11</v>
+      </c>
+      <c r="AA45" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27">
+      <c r="A46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" s="1">
+        <v>1</v>
+      </c>
+      <c r="C46" s="2">
+        <v>2010</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F46" s="1">
+        <v>14</v>
+      </c>
+      <c r="G46" s="1">
+        <v>294</v>
+      </c>
+      <c r="H46" s="1">
+        <v>432</v>
+      </c>
+      <c r="I46" s="1">
+        <v>4182</v>
+      </c>
+      <c r="J46" s="1">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="K46" s="1">
+        <v>14.2</v>
+      </c>
+      <c r="L46" s="1">
+        <v>298.7</v>
+      </c>
+      <c r="N46" s="1">
+        <v>50</v>
+      </c>
+      <c r="P46" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q46" s="1">
+        <v>85</v>
+      </c>
+      <c r="R46" s="1">
+        <v>125.2</v>
+      </c>
+      <c r="S46" s="1">
+        <v>32</v>
+      </c>
+      <c r="T46" s="1">
+        <v>-48</v>
+      </c>
+      <c r="U46" s="1">
+        <v>-1.5</v>
+      </c>
+      <c r="V46" s="1">
+        <v>-3.4</v>
+      </c>
+      <c r="W46" s="1">
+        <v>11</v>
+      </c>
+      <c r="Y46" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z46" s="1">
+        <v>12</v>
+      </c>
+      <c r="AA46" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27">
+      <c r="A47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1</v>
+      </c>
+      <c r="C47" s="2">
+        <v>2009</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F47" s="1">
+        <v>9</v>
+      </c>
+      <c r="G47" s="1">
+        <v>23</v>
+      </c>
+      <c r="H47" s="1">
+        <v>35</v>
+      </c>
+      <c r="I47" s="1">
+        <v>205</v>
+      </c>
+      <c r="J47" s="1">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="K47" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="L47" s="1">
+        <v>22.8</v>
+      </c>
+      <c r="N47" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q47" s="1">
+        <v>45</v>
+      </c>
+      <c r="R47" s="1">
+        <v>100.3</v>
+      </c>
+      <c r="S47" s="1">
+        <v>13</v>
+      </c>
+      <c r="T47" s="1">
+        <v>43</v>
+      </c>
+      <c r="U47" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="V47" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="W47" s="1">
+        <v>9</v>
+      </c>
+      <c r="Z47" s="1">
+        <v>8</v>
+      </c>
+      <c r="AA47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27">
+      <c r="A48" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1</v>
+      </c>
+      <c r="C48" s="2">
+        <v>2012</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F48" s="1">
+        <v>13</v>
+      </c>
+      <c r="G48" s="1">
+        <v>156</v>
+      </c>
+      <c r="H48" s="1">
+        <v>291</v>
+      </c>
+      <c r="I48" s="1">
+        <v>2144</v>
+      </c>
+      <c r="J48" s="1">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="K48" s="1">
+        <v>13.7</v>
+      </c>
+      <c r="L48" s="1">
+        <v>164.9</v>
+      </c>
+      <c r="N48" s="1">
+        <v>24</v>
+      </c>
+      <c r="P48" s="1">
+        <v>9</v>
+      </c>
+      <c r="Q48" s="1">
+        <v>78</v>
+      </c>
+      <c r="R48" s="1">
+        <v>92.1</v>
+      </c>
+      <c r="S48" s="1">
+        <v>89</v>
+      </c>
+      <c r="T48" s="1">
+        <v>436</v>
+      </c>
+      <c r="U48" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="V48" s="1">
+        <v>33.5</v>
+      </c>
+      <c r="W48" s="1">
+        <v>31</v>
+      </c>
+      <c r="Y48" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z48" s="1">
+        <v>10</v>
+      </c>
+      <c r="AA48" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27">
+      <c r="A49" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1</v>
+      </c>
+      <c r="C49" s="2">
+        <v>2011</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1">
+        <v>10</v>
+      </c>
+      <c r="G49" s="1">
+        <v>171</v>
+      </c>
+      <c r="H49" s="1">
+        <v>341</v>
+      </c>
+      <c r="I49" s="1">
+        <v>2164</v>
+      </c>
+      <c r="J49" s="1">
+        <v>0.501</v>
+      </c>
+      <c r="K49" s="1">
+        <v>12.7</v>
+      </c>
+      <c r="L49" s="1">
+        <v>216.4</v>
+      </c>
+      <c r="N49" s="1">
+        <v>20</v>
+      </c>
+      <c r="P49" s="1">
+        <v>16</v>
+      </c>
+      <c r="Q49" s="1">
+        <v>83</v>
+      </c>
+      <c r="R49" s="1">
+        <v>70.3</v>
+      </c>
+      <c r="S49" s="1">
+        <v>42</v>
+      </c>
+      <c r="T49" s="1">
+        <v>38</v>
+      </c>
+      <c r="U49" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="V49" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="W49" s="1">
+        <v>20</v>
+      </c>
+      <c r="Y49" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z49" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA49" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27">
+      <c r="A50" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" s="1">
+        <v>1</v>
+      </c>
+      <c r="C50" s="2">
+        <v>2010</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F50" s="1">
+        <v>11</v>
+      </c>
+      <c r="G50" s="1">
+        <v>87</v>
+      </c>
+      <c r="H50" s="1">
+        <v>168</v>
+      </c>
+      <c r="I50" s="1">
+        <v>1165</v>
+      </c>
+      <c r="J50" s="1">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="K50" s="1">
+        <v>13.4</v>
+      </c>
+      <c r="L50" s="1">
+        <v>105.9</v>
+      </c>
+      <c r="N50" s="1">
+        <v>11</v>
+      </c>
+      <c r="P50" s="1">
+        <v>8</v>
+      </c>
+      <c r="Q50" s="1">
+        <v>90</v>
+      </c>
+      <c r="R50" s="1">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="S50" s="1">
+        <v>28</v>
+      </c>
+      <c r="T50" s="1">
+        <v>-44</v>
+      </c>
+      <c r="U50" s="1">
+        <v>-1.6</v>
+      </c>
+      <c r="V50" s="1">
+        <v>-4</v>
+      </c>
+      <c r="W50" s="1">
+        <v>20</v>
+      </c>
+      <c r="Z50" s="1">
+        <v>7</v>
+      </c>
+      <c r="AA50" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27">
+      <c r="A51" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1</v>
+      </c>
+      <c r="C51" s="2">
+        <v>2012</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F51" s="1">
+        <v>6</v>
+      </c>
+      <c r="G51" s="1">
+        <v>61</v>
+      </c>
+      <c r="H51" s="1">
+        <v>113</v>
+      </c>
+      <c r="I51" s="1">
+        <v>738</v>
+      </c>
+      <c r="J51" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="K51" s="1">
+        <v>12.1</v>
+      </c>
+      <c r="L51" s="1">
+        <v>123</v>
+      </c>
+      <c r="N51" s="1">
+        <v>6</v>
+      </c>
+      <c r="P51" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q51" s="1">
+        <v>58</v>
+      </c>
+      <c r="R51" s="1">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="S51" s="1">
+        <v>19</v>
+      </c>
+      <c r="T51" s="1">
+        <v>-10</v>
+      </c>
+      <c r="U51" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="V51" s="1">
+        <v>-1.7</v>
+      </c>
+      <c r="W51" s="1">
+        <v>8</v>
+      </c>
+      <c r="Z51" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA51" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:27">
+      <c r="A52" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+      <c r="C52" s="2">
+        <v>2011</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1">
+        <v>12</v>
+      </c>
+      <c r="G52" s="1">
+        <v>121</v>
+      </c>
+      <c r="H52" s="1">
+        <v>235</v>
+      </c>
+      <c r="I52" s="1">
+        <v>1684</v>
+      </c>
+      <c r="J52" s="1">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="K52" s="1">
+        <v>13.9</v>
+      </c>
+      <c r="L52" s="1">
+        <v>140.30000000000001</v>
+      </c>
+      <c r="N52" s="1">
+        <v>19</v>
+      </c>
+      <c r="P52" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q52" s="1">
+        <v>65</v>
+      </c>
+      <c r="R52" s="1">
+        <v>89.4</v>
+      </c>
+      <c r="S52" s="1">
+        <v>74</v>
+      </c>
+      <c r="T52" s="1">
+        <v>150</v>
+      </c>
+      <c r="U52" s="1">
+        <v>2</v>
+      </c>
+      <c r="V52" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="W52" s="1">
+        <v>27</v>
+      </c>
+      <c r="Y52" s="1">
+        <v>6</v>
+      </c>
+      <c r="Z52" s="1">
+        <v>9</v>
+      </c>
+      <c r="AA52" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:27">
+      <c r="A53" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" s="1">
+        <v>1</v>
+      </c>
+      <c r="C53" s="2">
+        <v>2010</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F53" s="1">
+        <v>12</v>
+      </c>
+      <c r="G53" s="1">
+        <v>96</v>
+      </c>
+      <c r="H53" s="1">
+        <v>185</v>
+      </c>
+      <c r="I53" s="1">
+        <v>1142</v>
+      </c>
+      <c r="J53" s="1">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="K53" s="1">
+        <v>11.9</v>
+      </c>
+      <c r="L53" s="1">
+        <v>95.2</v>
+      </c>
+      <c r="N53" s="1">
+        <v>14</v>
+      </c>
+      <c r="P53" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q53" s="1">
+        <v>66</v>
+      </c>
+      <c r="R53" s="1">
+        <v>85</v>
+      </c>
+      <c r="S53" s="1">
+        <v>51</v>
+      </c>
+      <c r="T53" s="1">
+        <v>55</v>
+      </c>
+      <c r="U53" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="V53" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="W53" s="1">
+        <v>16</v>
+      </c>
+      <c r="Y53" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z53" s="1">
+        <v>9</v>
+      </c>
+      <c r="AA53" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:27">
+      <c r="A54" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54" s="1">
+        <v>1</v>
+      </c>
+      <c r="C54" s="2">
+        <v>2009</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F54" s="1">
+        <v>5</v>
+      </c>
+      <c r="G54" s="1">
+        <v>12</v>
+      </c>
+      <c r="H54" s="1">
+        <v>35</v>
+      </c>
+      <c r="I54" s="1">
+        <v>198</v>
+      </c>
+      <c r="J54" s="1">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="K54" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="L54" s="1">
+        <v>39.6</v>
+      </c>
+      <c r="N54" s="1">
+        <v>3</v>
+      </c>
+      <c r="P54" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q54" s="1">
+        <v>37</v>
+      </c>
+      <c r="R54" s="1">
+        <v>47.1</v>
+      </c>
+      <c r="S54" s="1">
+        <v>13</v>
+      </c>
+      <c r="T54" s="1">
+        <v>-25</v>
+      </c>
+      <c r="U54" s="1">
+        <v>-1.9</v>
+      </c>
+      <c r="V54" s="1">
+        <v>-5</v>
+      </c>
+      <c r="W54" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z54" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27">
+      <c r="A55" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55" s="1">
+        <v>1</v>
+      </c>
+      <c r="C55" s="2">
+        <v>2012</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F55" s="1">
+        <v>4</v>
+      </c>
+      <c r="G55" s="1">
+        <v>34</v>
+      </c>
+      <c r="H55" s="1">
+        <v>59</v>
+      </c>
+      <c r="I55" s="1">
+        <v>396</v>
+      </c>
+      <c r="J55" s="1">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="K55" s="1">
+        <v>11.6</v>
+      </c>
+      <c r="L55" s="1">
+        <v>99</v>
+      </c>
+      <c r="N55" s="1">
+        <v>7</v>
+      </c>
+      <c r="P55" s="1">
+        <v>2</v>
+      </c>
+      <c r="R55" s="1">
+        <v>103.5</v>
+      </c>
+      <c r="Y55" s="1">
+        <v>6</v>
+      </c>
+      <c r="Z55" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA55" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:27">
+      <c r="A56" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" s="1">
+        <v>1</v>
+      </c>
+      <c r="C56" s="2">
+        <v>2011</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F56" s="1">
+        <v>10</v>
+      </c>
+      <c r="G56" s="1">
+        <v>168</v>
+      </c>
+      <c r="H56" s="1">
+        <v>308</v>
+      </c>
+      <c r="I56" s="1">
+        <v>2484</v>
+      </c>
+      <c r="J56" s="1">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="K56" s="1">
+        <v>14.8</v>
+      </c>
+      <c r="L56" s="1">
+        <v>248.4</v>
+      </c>
+      <c r="N56" s="1">
+        <v>26</v>
+      </c>
+      <c r="P56" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q56" s="1">
+        <v>86</v>
+      </c>
+      <c r="R56" s="1">
+        <v>99.8</v>
+      </c>
+      <c r="S56" s="1">
+        <v>93</v>
+      </c>
+      <c r="T56" s="1">
+        <v>183</v>
+      </c>
+      <c r="U56" s="1">
+        <v>2</v>
+      </c>
+      <c r="V56" s="1">
+        <v>18.3</v>
+      </c>
+      <c r="W56" s="1">
+        <v>27</v>
+      </c>
+      <c r="Y56" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z56" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA56" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27">
+      <c r="A57" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" s="1">
+        <v>1</v>
+      </c>
+      <c r="C57" s="2">
+        <v>2010</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F57" s="1">
+        <v>7</v>
+      </c>
+      <c r="G57" s="1">
+        <v>69</v>
+      </c>
+      <c r="H57" s="1">
+        <v>125</v>
+      </c>
+      <c r="I57" s="1">
+        <v>1082</v>
+      </c>
+      <c r="J57" s="1">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="K57" s="1">
+        <v>15.7</v>
+      </c>
+      <c r="L57" s="1">
+        <v>154.6</v>
+      </c>
+      <c r="N57" s="1">
+        <v>13</v>
+      </c>
+      <c r="P57" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q57" s="1">
+        <v>56</v>
+      </c>
+      <c r="R57" s="1">
+        <v>112.2</v>
+      </c>
+      <c r="S57" s="1">
+        <v>22</v>
+      </c>
+      <c r="T57" s="1">
+        <v>2</v>
+      </c>
+      <c r="U57" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="V57" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="W57" s="1">
+        <v>9</v>
+      </c>
+      <c r="Y57" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z57" s="1">
+        <v>7</v>
+      </c>
+      <c r="AA57" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:27">
+      <c r="A58" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="1">
+        <v>1</v>
+      </c>
+      <c r="C58" s="2">
+        <v>2012</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F58" s="1">
+        <v>4</v>
+      </c>
+      <c r="G58" s="1">
+        <v>39</v>
+      </c>
+      <c r="H58" s="1">
+        <v>77</v>
+      </c>
+      <c r="I58" s="1">
+        <v>448</v>
+      </c>
+      <c r="J58" s="1">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="K58" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="L58" s="1">
+        <v>112</v>
+      </c>
+      <c r="N58" s="1">
+        <v>5</v>
+      </c>
+      <c r="P58" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q58" s="1">
+        <v>41</v>
+      </c>
+      <c r="R58" s="1">
+        <v>63.1</v>
+      </c>
+      <c r="S58" s="1">
+        <v>7</v>
+      </c>
+      <c r="T58" s="1">
+        <v>90</v>
+      </c>
+      <c r="U58" s="1">
+        <v>12.9</v>
+      </c>
+      <c r="V58" s="1">
+        <v>22.5</v>
+      </c>
+      <c r="W58" s="1">
+        <v>19</v>
+      </c>
+      <c r="Y58" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z58" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA58" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:27">
+      <c r="A59" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+      <c r="C59" s="2">
+        <v>2011</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F59" s="1">
+        <v>12</v>
+      </c>
+      <c r="G59" s="1">
+        <v>124</v>
+      </c>
+      <c r="H59" s="1">
+        <v>205</v>
+      </c>
+      <c r="I59" s="1">
+        <v>1686</v>
+      </c>
+      <c r="J59" s="1">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="K59" s="1">
+        <v>13.6</v>
+      </c>
+      <c r="L59" s="1">
+        <v>140.5</v>
+      </c>
+      <c r="N59" s="1">
+        <v>20</v>
+      </c>
+      <c r="P59" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q59" s="1">
+        <v>57</v>
+      </c>
+      <c r="R59" s="1">
+        <v>107.1</v>
+      </c>
+      <c r="S59" s="1">
+        <v>16</v>
+      </c>
+      <c r="T59" s="1">
+        <v>95</v>
+      </c>
+      <c r="U59" s="1">
+        <v>5.9</v>
+      </c>
+      <c r="V59" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="W59" s="1">
+        <v>22</v>
+      </c>
+      <c r="Y59" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z59" s="1">
+        <v>11</v>
+      </c>
+      <c r="AA59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:27">
+      <c r="A60" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="1">
+        <v>1</v>
+      </c>
+      <c r="C60" s="2">
+        <v>2010</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F60" s="1">
+        <v>12</v>
+      </c>
+      <c r="G60" s="1">
+        <v>95</v>
+      </c>
+      <c r="H60" s="1">
+        <v>171</v>
+      </c>
+      <c r="I60" s="1">
+        <v>1341</v>
+      </c>
+      <c r="J60" s="1">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="K60" s="1">
+        <v>14.1</v>
+      </c>
+      <c r="L60" s="1">
+        <v>111.8</v>
+      </c>
+      <c r="N60" s="1">
+        <v>15</v>
+      </c>
+      <c r="P60" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q60" s="1">
+        <v>57</v>
+      </c>
+      <c r="R60" s="1">
+        <v>95.7</v>
+      </c>
+      <c r="S60" s="1">
+        <v>10</v>
+      </c>
+      <c r="T60" s="1">
+        <v>36</v>
+      </c>
+      <c r="U60" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="V60" s="1">
+        <v>3</v>
+      </c>
+      <c r="W60" s="1">
+        <v>11</v>
+      </c>
+      <c r="Y60" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z60" s="1">
+        <v>11</v>
+      </c>
+      <c r="AA60" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27">
+      <c r="A61" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1">
+        <v>1</v>
+      </c>
+      <c r="C61" s="2">
+        <v>2009</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F61" s="1">
+        <v>1</v>
+      </c>
+      <c r="G61" s="1">
+        <v>1</v>
+      </c>
+      <c r="H61" s="1">
+        <v>3</v>
+      </c>
+      <c r="I61" s="1">
+        <v>6</v>
+      </c>
+      <c r="J61" s="1">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="K61" s="1">
+        <v>6</v>
+      </c>
+      <c r="L61" s="1">
+        <v>6</v>
+      </c>
+      <c r="P61" s="1">
+        <v>0</v>
+      </c>
+      <c r="R61" s="1">
+        <v>42.4</v>
+      </c>
+      <c r="Z61" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA61" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27">
+      <c r="A62" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1">
+        <v>1</v>
+      </c>
+      <c r="C62" s="2">
+        <v>2012</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F62" s="1">
+        <v>15</v>
+      </c>
+      <c r="G62" s="1">
+        <v>191</v>
+      </c>
+      <c r="H62" s="1">
+        <v>266</v>
+      </c>
+      <c r="I62" s="1">
+        <v>2881</v>
+      </c>
+      <c r="J62" s="1">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="K62" s="1">
+        <v>15.1</v>
+      </c>
+      <c r="L62" s="1">
+        <v>192.1</v>
+      </c>
+      <c r="N62" s="1">
+        <v>39</v>
+      </c>
+      <c r="P62" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q62" s="1">
+        <v>69</v>
+      </c>
+      <c r="R62" s="1">
+        <v>137.19999999999999</v>
+      </c>
+      <c r="S62" s="1">
+        <v>94</v>
+      </c>
+      <c r="T62" s="1">
+        <v>396</v>
+      </c>
+      <c r="U62" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="V62" s="1">
+        <v>26.4</v>
+      </c>
+      <c r="W62" s="1">
+        <v>33</v>
+      </c>
+      <c r="Y62" s="1">
+        <v>10</v>
+      </c>
+      <c r="Z62" s="1">
+        <v>14</v>
+      </c>
+      <c r="AA62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27">
+      <c r="A63" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B63" s="1">
+        <v>1</v>
+      </c>
+      <c r="C63" s="2">
+        <v>2011</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F63" s="1">
+        <v>14</v>
+      </c>
+      <c r="G63" s="1">
+        <v>211</v>
+      </c>
+      <c r="H63" s="1">
+        <v>339</v>
+      </c>
+      <c r="I63" s="1">
+        <v>3247</v>
+      </c>
+      <c r="J63" s="1">
+        <v>0.622</v>
+      </c>
+      <c r="K63" s="1">
+        <v>15.4</v>
+      </c>
+      <c r="L63" s="1">
+        <v>231.9</v>
+      </c>
+      <c r="N63" s="1">
+        <v>34</v>
+      </c>
+      <c r="P63" s="1">
+        <v>11</v>
+      </c>
+      <c r="Q63" s="1">
+        <v>76</v>
+      </c>
+      <c r="R63" s="1">
+        <v>113.8</v>
+      </c>
+      <c r="S63" s="1">
+        <v>102</v>
+      </c>
+      <c r="T63" s="1">
+        <v>587</v>
+      </c>
+      <c r="U63" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="V63" s="1">
+        <v>41.9</v>
+      </c>
+      <c r="W63" s="1">
+        <v>41</v>
+      </c>
+      <c r="Y63" s="1">
+        <v>11</v>
+      </c>
+      <c r="Z63" s="1">
+        <v>11</v>
+      </c>
+      <c r="AA63" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:27">
+      <c r="A64" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B64" s="1">
+        <v>1</v>
+      </c>
+      <c r="C64" s="2">
+        <v>2010</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F64" s="1">
+        <v>12</v>
+      </c>
+      <c r="G64" s="1">
+        <v>200</v>
+      </c>
+      <c r="H64" s="1">
+        <v>317</v>
+      </c>
+      <c r="I64" s="1">
+        <v>2597</v>
+      </c>
+      <c r="J64" s="1">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="K64" s="1">
+        <v>13</v>
+      </c>
+      <c r="L64" s="1">
+        <v>216.4</v>
+      </c>
+      <c r="N64" s="1">
+        <v>23</v>
+      </c>
+      <c r="P64" s="1">
+        <v>9</v>
+      </c>
+      <c r="Q64" s="1">
+        <v>53</v>
+      </c>
+      <c r="R64" s="1">
+        <v>101.2</v>
+      </c>
+      <c r="S64" s="1">
+        <v>81</v>
+      </c>
+      <c r="T64" s="1">
+        <v>172</v>
+      </c>
+      <c r="U64" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="V64" s="1">
+        <v>14.3</v>
+      </c>
+      <c r="W64" s="1">
+        <v>9</v>
+      </c>
+      <c r="Y64" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z64" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA64" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:27">
+      <c r="A65" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B65" s="1">
+        <v>1</v>
+      </c>
+      <c r="C65" s="2">
+        <v>2009</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F65" s="1">
+        <v>4</v>
+      </c>
+      <c r="G65" s="1">
+        <v>8</v>
+      </c>
+      <c r="H65" s="1">
+        <v>12</v>
+      </c>
+      <c r="I65" s="1">
+        <v>130</v>
+      </c>
+      <c r="J65" s="1">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="K65" s="1">
+        <v>16.3</v>
+      </c>
+      <c r="L65" s="1">
+        <v>32.5</v>
+      </c>
+      <c r="N65" s="1">
+        <v>2</v>
+      </c>
+      <c r="P65" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q65" s="1">
+        <v>55</v>
+      </c>
+      <c r="R65" s="1">
+        <v>107.6</v>
+      </c>
+      <c r="S65" s="1">
+        <v>4</v>
+      </c>
+      <c r="T65" s="1">
+        <v>54</v>
+      </c>
+      <c r="U65" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="V65" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="W65" s="1">
+        <v>20</v>
+      </c>
+      <c r="Z65" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA65" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>